<commit_message>
modificación de la lista de componentes
</commit_message>
<xml_diff>
--- a/Librería de componentes.xlsx
+++ b/Librería de componentes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YUNELY\Desktop\ITLA\Décimo segundo cuatrimestre\Electiva Mecatrónica - Diseño Mecatrónico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB887BD6-B1B9-442B-9DEC-8AFACA89A4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED01097-00BC-4C9F-847B-085CE8A42C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{49458E5D-DEEC-430E-940B-19D27B1F3765}"/>
   </bookViews>
@@ -1189,7 +1189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1198,55 +1198,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="39">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1310,6 +1269,9 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1333,9 +1295,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1381,6 +1340,9 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1404,9 +1366,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1458,6 +1417,9 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1481,6 +1443,15 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1516,6 +1487,34 @@
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1530,67 +1529,67 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{36E12380-37CE-400D-B2F7-9E38CEE17764}" name="Tabla20" displayName="Tabla20" ref="A1:G42" totalsRowShown="0" headerRowDxfId="32" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{36E12380-37CE-400D-B2F7-9E38CEE17764}" name="Tabla20" displayName="Tabla20" ref="A1:G42" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
   <autoFilter ref="A1:G42" xr:uid="{36E12380-37CE-400D-B2F7-9E38CEE17764}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{796517A2-73C5-4AF6-A4B5-753C303D8BE0}" name="Número de parte" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{3D9D4BAA-0B2E-4274-A6C0-FD18ED42728F}" name="Valor (Ω)" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{71C72941-6CCE-4564-89D6-759C10E7E45F}" name="Tolerancia (%)" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{74C25F89-FC78-43D5-BA38-77C1FEF1B16D}" name="Potencia (W)" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{BAD468FB-A718-4770-868F-253225E6AFAA}" name="Coeficiente de tempratura (PPM/C)" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{2CEBA80D-0FDB-4E1D-9BA1-BE811ACC912B}" name="Fabricante" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{F4BC416D-0CF7-483A-8FDF-B0E6E2C4B348}" name="Agregado" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{796517A2-73C5-4AF6-A4B5-753C303D8BE0}" name="Número de parte" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{3D9D4BAA-0B2E-4274-A6C0-FD18ED42728F}" name="Valor (Ω)" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{71C72941-6CCE-4564-89D6-759C10E7E45F}" name="Tolerancia (%)" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{74C25F89-FC78-43D5-BA38-77C1FEF1B16D}" name="Potencia (W)" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{BAD468FB-A718-4770-868F-253225E6AFAA}" name="Coeficiente de tempratura (PPM/C)" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{2CEBA80D-0FDB-4E1D-9BA1-BE811ACC912B}" name="Fabricante" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{F4BC416D-0CF7-483A-8FDF-B0E6E2C4B348}" name="Agregado" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{094A1CDA-BED8-4FA8-B90D-2F30FF900E97}" name="Tabla21" displayName="Tabla21" ref="A1:I65" totalsRowShown="0" headerRowDxfId="21" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{094A1CDA-BED8-4FA8-B90D-2F30FF900E97}" name="Tabla21" displayName="Tabla21" ref="A1:I65" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A1:I65" xr:uid="{094A1CDA-BED8-4FA8-B90D-2F30FF900E97}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{F9621106-4CBA-485E-A6A7-F959B9D5BAA4}" name="Número de parte" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{727F9A12-8C4D-45B2-BA2C-2741DB2339B7}" name="Valor (F)" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{0B9ADF9C-C80E-439B-8F1B-45EB641545E9}" name="Tolerancia (%)" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{1D7059B7-9582-4653-8FD0-0833B6574001}" name="Voltaje (v)" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{6A418381-1452-4BB9-B8E9-C7D591A975F4}" name="Tipo de voltaje" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{B7BE1B50-568D-415D-8701-DB0BF62EA996}" name="Vida (horas)" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{CD39A474-7F91-47B0-A6C8-DA36A387B50D}" name="Tipo" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{F8C3E44C-4CFE-45BA-A2C5-6E552212B32F}" name="Fabricante" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{AED96924-7F26-4825-8814-2F9A40A1BDD9}" name="Agregado" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{F9621106-4CBA-485E-A6A7-F959B9D5BAA4}" name="Número de parte" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{727F9A12-8C4D-45B2-BA2C-2741DB2339B7}" name="Valor (F)" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{0B9ADF9C-C80E-439B-8F1B-45EB641545E9}" name="Tolerancia (%)" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{1D7059B7-9582-4653-8FD0-0833B6574001}" name="Voltaje (v)" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{6A418381-1452-4BB9-B8E9-C7D591A975F4}" name="Tipo de voltaje" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{B7BE1B50-568D-415D-8701-DB0BF62EA996}" name="Vida (horas)" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{CD39A474-7F91-47B0-A6C8-DA36A387B50D}" name="Tipo" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{F8C3E44C-4CFE-45BA-A2C5-6E552212B32F}" name="Fabricante" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{AED96924-7F26-4825-8814-2F9A40A1BDD9}" name="Agregado" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{81AEC8DF-CB6F-4A4A-A3CD-ACA34366D852}" name="Tabla22" displayName="Tabla22" ref="A1:G68" totalsRowShown="0" headerRowDxfId="12" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{81AEC8DF-CB6F-4A4A-A3CD-ACA34366D852}" name="Tabla22" displayName="Tabla22" ref="A1:G68" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A1:G68" xr:uid="{81AEC8DF-CB6F-4A4A-A3CD-ACA34366D852}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{21F9D534-4783-4EA9-A890-5356620CE1BC}" name="Número de parte" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{E9668112-3805-4143-B6C1-87C87AB0E5A0}" name="Valor (H)" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{8F8A61A6-8021-4596-951C-765370CEAB10}" name="Tolerancia (%)" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{0C85D6BC-C464-41C2-9A72-6D06275FE232}" name="Corriente (A)" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{32972288-40B5-4DD9-9215-18531D5D3838}" name="Tipo" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{37F575D6-0780-47B8-924C-3AAA92F10605}" name="Fabricante" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{7708C74C-21CF-4A9B-85E2-21F6925251D1}" name="Agregado" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{21F9D534-4783-4EA9-A890-5356620CE1BC}" name="Número de parte" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{E9668112-3805-4143-B6C1-87C87AB0E5A0}" name="Valor (H)" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{8F8A61A6-8021-4596-951C-765370CEAB10}" name="Tolerancia (%)" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{0C85D6BC-C464-41C2-9A72-6D06275FE232}" name="Corriente (A)" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{32972288-40B5-4DD9-9215-18531D5D3838}" name="Tipo" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{37F575D6-0780-47B8-924C-3AAA92F10605}" name="Fabricante" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{7708C74C-21CF-4A9B-85E2-21F6925251D1}" name="Agregado" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{F9ABAB21-2534-4602-B505-BC400EFEBC75}" name="Tabla23" displayName="Tabla23" ref="A1:H19" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{F9ABAB21-2534-4602-B505-BC400EFEBC75}" name="Tabla23" displayName="Tabla23" ref="A1:H19" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:H19" xr:uid="{F9ABAB21-2534-4602-B505-BC400EFEBC75}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{7261B210-8024-41E8-A775-16C44D2F1D76}" name="Número de parte" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{4DFEE4F8-7545-4360-A64D-34145DA5CC52}" name="Tecnología" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{78713A6B-7197-45D9-A9B6-7011366C51D0}" name="Polaridad" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{AC2D5852-5116-4A1D-8B2F-784159912DDC}" name="Vgs-th (v)" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{CC022B58-04A3-4687-9C74-5DC2DB6801FD}" name="Id (A)" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{8D220D3F-D36D-4D32-8C07-F4720A934B43}" name="Potencia (W)" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{A536371A-B0C9-4273-86B9-3C8562768D0C}" name="Fabricante" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{C04B2730-F623-48A3-83DC-3C4DCC77E821}" name="Agregado" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{7261B210-8024-41E8-A775-16C44D2F1D76}" name="Número de parte" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{4DFEE4F8-7545-4360-A64D-34145DA5CC52}" name="Tecnología" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{78713A6B-7197-45D9-A9B6-7011366C51D0}" name="Polaridad" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{AC2D5852-5116-4A1D-8B2F-784159912DDC}" name="Vgs-th (v)" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{CC022B58-04A3-4687-9C74-5DC2DB6801FD}" name="Id (A)" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{8D220D3F-D36D-4D32-8C07-F4720A934B43}" name="Potencia (W)" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{A536371A-B0C9-4273-86B9-3C8562768D0C}" name="Fabricante" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{C04B2730-F623-48A3-83DC-3C4DCC77E821}" name="Agregado" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1916,7 +1915,8 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2919,7 +2919,8 @@
   <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2935,7 +2936,7 @@
     <col min="9" max="9" width="18.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4842,7 +4843,8 @@
   <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView zoomScale="132" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4856,7 +4858,7 @@
     <col min="7" max="7" width="17" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -6442,7 +6444,8 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6457,7 +6460,7 @@
     <col min="8" max="8" width="15.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Clase 5 y 6 y actualización de la librería de componentes
</commit_message>
<xml_diff>
--- a/Librería de componentes.xlsx
+++ b/Librería de componentes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YUNELY\Desktop\ITLA\Décimo segundo cuatrimestre\Electiva Mecatrónica - Diseño Mecatrónico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671D9214-453D-4514-BA33-0FD20D82AF5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A094717F-15D4-4A5E-8A8C-7AB34A223239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{49458E5D-DEEC-430E-940B-19D27B1F3765}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{49458E5D-DEEC-430E-940B-19D27B1F3765}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistencias" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Transistores" sheetId="4" r:id="rId4"/>
     <sheet name="OPAMPs" sheetId="5" r:id="rId5"/>
     <sheet name="LEDs" sheetId="6" r:id="rId6"/>
+    <sheet name="No clasificados" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="486">
   <si>
     <t>Número de parte</t>
   </si>
@@ -1236,15 +1237,6 @@
     <t>1.5m</t>
   </si>
   <si>
-    <t>MAX492ESA+T</t>
-  </si>
-  <si>
-    <t>500u</t>
-  </si>
-  <si>
-    <t>60n</t>
-  </si>
-  <si>
     <t>AD648KRZ</t>
   </si>
   <si>
@@ -1299,9 +1291,6 @@
     <t>28m</t>
   </si>
   <si>
-    <t>MAX494ESD+T</t>
-  </si>
-  <si>
     <t>AD8544WARZ-R7</t>
   </si>
   <si>
@@ -1365,9 +1354,6 @@
     <t>Verde</t>
   </si>
   <si>
-    <t>LY P47K-J1L2-26</t>
-  </si>
-  <si>
     <t>Amarillo</t>
   </si>
   <si>
@@ -1465,13 +1451,85 @@
   </si>
   <si>
     <t>4.6m</t>
+  </si>
+  <si>
+    <t>MAX4402AKA/V+T</t>
+  </si>
+  <si>
+    <t>800k</t>
+  </si>
+  <si>
+    <t>100f</t>
+  </si>
+  <si>
+    <t>SSSF021500</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>B3SL-1022P</t>
+  </si>
+  <si>
+    <t>Botón</t>
+  </si>
+  <si>
+    <t>12401832E402A</t>
+  </si>
+  <si>
+    <t>Conector USB</t>
+  </si>
+  <si>
+    <t>WJ128V-5.0-6P</t>
+  </si>
+  <si>
+    <t>Screw terminal block</t>
+  </si>
+  <si>
+    <t>3296W-1-203LF</t>
+  </si>
+  <si>
+    <t>Potenciómetro</t>
+  </si>
+  <si>
+    <t>RLB1014-104KL</t>
+  </si>
+  <si>
+    <t>Bobina de poder</t>
+  </si>
+  <si>
+    <t>RVT1H470M0607</t>
+  </si>
+  <si>
+    <t>Capacitor bulk</t>
+  </si>
+  <si>
+    <t>Conector XT30</t>
+  </si>
+  <si>
+    <t>XT30UPB-M</t>
+  </si>
+  <si>
+    <t>OP496GSZ</t>
+  </si>
+  <si>
+    <t>450k</t>
+  </si>
+  <si>
+    <t>300u</t>
+  </si>
+  <si>
+    <t>50n</t>
+  </si>
+  <si>
+    <t>LY T67K-J2M1-26</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1515,6 +1573,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF222222"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1536,7 +1606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1554,6 +1624,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2401,9 +2474,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEAEBF3B-4C72-4C22-8C79-512894A2A873}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2460,12 +2533,12 @@
         <v>74</v>
       </c>
       <c r="G2" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="B3" s="3">
         <v>100</v>
@@ -2483,7 +2556,7 @@
         <v>74</v>
       </c>
       <c r="G3" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -2506,7 +2579,7 @@
         <v>74</v>
       </c>
       <c r="G4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -2529,7 +2602,7 @@
         <v>74</v>
       </c>
       <c r="G5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -2552,7 +2625,7 @@
         <v>74</v>
       </c>
       <c r="G6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -2575,7 +2648,7 @@
         <v>74</v>
       </c>
       <c r="G7" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -2598,7 +2671,7 @@
         <v>74</v>
       </c>
       <c r="G8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -2621,7 +2694,7 @@
         <v>74</v>
       </c>
       <c r="G9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -2644,7 +2717,7 @@
         <v>74</v>
       </c>
       <c r="G10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -2667,7 +2740,7 @@
         <v>74</v>
       </c>
       <c r="G11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -2690,7 +2763,7 @@
         <v>74</v>
       </c>
       <c r="G12" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -2713,7 +2786,7 @@
         <v>74</v>
       </c>
       <c r="G13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -2736,7 +2809,7 @@
         <v>74</v>
       </c>
       <c r="G14" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -2759,7 +2832,7 @@
         <v>74</v>
       </c>
       <c r="G15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -2782,7 +2855,7 @@
         <v>74</v>
       </c>
       <c r="G16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -2805,7 +2878,7 @@
         <v>74</v>
       </c>
       <c r="G17" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -2828,7 +2901,7 @@
         <v>74</v>
       </c>
       <c r="G18" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -2851,7 +2924,7 @@
         <v>74</v>
       </c>
       <c r="G19" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -2874,7 +2947,7 @@
         <v>74</v>
       </c>
       <c r="G20" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -2897,7 +2970,7 @@
         <v>74</v>
       </c>
       <c r="G21" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -2920,7 +2993,7 @@
         <v>74</v>
       </c>
       <c r="G22" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -2943,7 +3016,7 @@
         <v>74</v>
       </c>
       <c r="G23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -2966,7 +3039,7 @@
         <v>74</v>
       </c>
       <c r="G24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -2989,7 +3062,7 @@
         <v>74</v>
       </c>
       <c r="G25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -3012,7 +3085,7 @@
         <v>74</v>
       </c>
       <c r="G26" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -3035,7 +3108,7 @@
         <v>74</v>
       </c>
       <c r="G27" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -3058,7 +3131,7 @@
         <v>74</v>
       </c>
       <c r="G28" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -3081,7 +3154,7 @@
         <v>74</v>
       </c>
       <c r="G29" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -3104,7 +3177,7 @@
         <v>74</v>
       </c>
       <c r="G30" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -3127,7 +3200,7 @@
         <v>74</v>
       </c>
       <c r="G31" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -3150,7 +3223,7 @@
         <v>74</v>
       </c>
       <c r="G32" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -3173,7 +3246,7 @@
         <v>74</v>
       </c>
       <c r="G33" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -3196,7 +3269,7 @@
         <v>74</v>
       </c>
       <c r="G34" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -3219,7 +3292,7 @@
         <v>74</v>
       </c>
       <c r="G35" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -3242,7 +3315,7 @@
         <v>74</v>
       </c>
       <c r="G36" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -3265,7 +3338,7 @@
         <v>74</v>
       </c>
       <c r="G37" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -3288,7 +3361,7 @@
         <v>74</v>
       </c>
       <c r="G38" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -3311,7 +3384,7 @@
         <v>74</v>
       </c>
       <c r="G39" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -3334,7 +3407,7 @@
         <v>74</v>
       </c>
       <c r="G40" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -3357,7 +3430,7 @@
         <v>74</v>
       </c>
       <c r="G41" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -3380,7 +3453,7 @@
         <v>74</v>
       </c>
       <c r="G42" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3405,9 +3478,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C205CF36-A0B2-46BE-A22B-1B8CB93B9542}">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I57" sqref="I57"/>
+    <sheetView zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4957,7 +5030,7 @@
         <v>82</v>
       </c>
       <c r="I53" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
@@ -4986,7 +5059,7 @@
         <v>82</v>
       </c>
       <c r="I54" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
@@ -5015,7 +5088,7 @@
         <v>82</v>
       </c>
       <c r="I55" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
@@ -5044,7 +5117,7 @@
         <v>82</v>
       </c>
       <c r="I56" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
@@ -5073,7 +5146,7 @@
         <v>82</v>
       </c>
       <c r="I57" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
@@ -5131,7 +5204,7 @@
         <v>82</v>
       </c>
       <c r="I59" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
@@ -5160,7 +5233,7 @@
         <v>82</v>
       </c>
       <c r="I60" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
@@ -5189,7 +5262,7 @@
         <v>82</v>
       </c>
       <c r="I61" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
@@ -5247,7 +5320,7 @@
         <v>82</v>
       </c>
       <c r="I63" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
@@ -5255,7 +5328,7 @@
         <v>206</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="C64" s="3">
         <v>20</v>
@@ -5276,7 +5349,7 @@
         <v>82</v>
       </c>
       <c r="I64" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
@@ -5284,7 +5357,7 @@
         <v>207</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="C65" s="3">
         <v>20</v>
@@ -5305,7 +5378,7 @@
         <v>82</v>
       </c>
       <c r="I65" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -5329,7 +5402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85404F1D-3E5E-4D66-9A35-71A1D2CD5641}">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView zoomScale="74" workbookViewId="0">
+    <sheetView zoomScale="131" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
@@ -6930,9 +7003,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D930AD8F-3E56-42DC-B88D-0B20D209FC4D}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView zoomScale="121" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="136" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7464,8 +7537,8 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView zoomScale="109" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7760,7 +7833,7 @@
         <v>363</v>
       </c>
       <c r="K8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -7795,33 +7868,33 @@
         <v>363</v>
       </c>
       <c r="K9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>390</v>
+        <v>462</v>
       </c>
       <c r="B10" s="3">
         <v>2</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>233</v>
+        <v>463</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>391</v>
+        <v>305</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>392</v>
+        <v>464</v>
       </c>
       <c r="G10" s="3">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="H10" s="3">
-        <v>2.7</v>
+        <v>2.5</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>362</v>
@@ -7830,12 +7903,12 @@
         <v>363</v>
       </c>
       <c r="K10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B11" s="3">
         <v>2</v>
@@ -7850,7 +7923,7 @@
         <v>203</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G11" s="3">
         <v>76</v>
@@ -7870,7 +7943,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
@@ -7905,7 +7978,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B13" s="3">
         <v>2</v>
@@ -7920,7 +7993,7 @@
         <v>377</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="G13" s="3">
         <v>90</v>
@@ -7935,12 +8008,12 @@
         <v>363</v>
       </c>
       <c r="K13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B14" s="3">
         <v>2</v>
@@ -7955,7 +8028,7 @@
         <v>305</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="G14" s="3">
         <v>90</v>
@@ -7975,13 +8048,13 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B15" s="3">
         <v>2</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D15" s="3">
         <v>650</v>
@@ -7990,7 +8063,7 @@
         <v>305</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="G15" s="3">
         <v>80</v>
@@ -8010,22 +8083,22 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B16" s="3">
         <v>3</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D16" s="3">
         <v>170</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="G16" s="3">
         <v>88</v>
@@ -8040,27 +8113,27 @@
         <v>363</v>
       </c>
       <c r="K16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B17" s="3">
         <v>3</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D17" s="3">
         <v>210</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="G17" s="3">
         <v>88</v>
@@ -8080,7 +8153,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B18" s="3">
         <v>4</v>
@@ -8089,7 +8162,7 @@
         <v>387</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>195</v>
@@ -8110,33 +8183,33 @@
         <v>363</v>
       </c>
       <c r="K18" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>411</v>
+        <v>481</v>
       </c>
       <c r="B19" s="3">
         <v>4</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>368</v>
+        <v>482</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>391</v>
+        <v>483</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>392</v>
+        <v>484</v>
       </c>
       <c r="G19" s="3">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H19" s="3">
-        <v>2.7</v>
+        <v>3</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>362</v>
@@ -8145,12 +8218,12 @@
         <v>363</v>
       </c>
       <c r="K19" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B20" s="3">
         <v>4</v>
@@ -8159,13 +8232,13 @@
         <v>70</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>305</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="G20" s="3">
         <v>45</v>
@@ -8185,7 +8258,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B21" s="3">
         <v>4</v>
@@ -8220,7 +8293,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="B22" s="3">
         <v>4</v>
@@ -8235,7 +8308,7 @@
         <v>377</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="G22" s="3">
         <v>90</v>
@@ -8255,22 +8328,22 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="B23" s="3">
         <v>4</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D23" s="3">
         <v>62</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="G23" s="3">
         <v>80</v>
@@ -8290,22 +8363,22 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="B24" s="3">
         <v>4</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D24" s="3">
         <v>170</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="G24" s="3">
         <v>88</v>
@@ -8334,8 +8407,9 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -8344,9 +8418,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A95F01-B128-436C-9F73-5C18FF680B8D}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="129" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8368,13 +8442,13 @@
         <v>77</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>73</v>
@@ -8385,13 +8459,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>271</v>
@@ -8400,7 +8474,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
@@ -8408,13 +8482,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>426</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>430</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>271</v>
@@ -8423,21 +8497,21 @@
         <v>2.7</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G3" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>271</v>
@@ -8446,44 +8520,44 @@
         <v>1.9</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G4" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>433</v>
+        <v>485</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>271</v>
+        <v>439</v>
       </c>
       <c r="E5" s="3">
-        <v>1.8</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G5" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>271</v>
@@ -8492,21 +8566,21 @@
         <v>2.7</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>271</v>
@@ -8515,21 +8589,21 @@
         <v>1.8</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G7" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>271</v>
@@ -8538,21 +8612,21 @@
         <v>1.8</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G8" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>271</v>
@@ -8561,44 +8635,44 @@
         <v>1.8</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="E10" s="3">
         <v>2.4</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>271</v>
@@ -8607,21 +8681,21 @@
         <v>1.9</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>240</v>
@@ -8630,44 +8704,44 @@
         <v>2.7</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="E13" s="3">
         <v>2.8</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G13" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>271</v>
@@ -8676,21 +8750,21 @@
         <v>2.8</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G14" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>259</v>
@@ -8699,21 +8773,21 @@
         <v>2.7</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>255</v>
@@ -8722,67 +8796,67 @@
         <v>3</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G16" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="E17" s="3">
         <v>3.2</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="E18" s="3">
         <v>1.6</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G18" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>309</v>
@@ -8791,10 +8865,10 @@
         <v>1.5</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G19" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -8812,4 +8886,87 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{081F05B9-1E94-428E-A64E-FFAE895AC322}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="2" max="2" width="29.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>465</v>
+      </c>
+      <c r="B1" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="B2" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="B3" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="B4" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="B5" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>475</v>
+      </c>
+      <c r="B6" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>477</v>
+      </c>
+      <c r="B7" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>480</v>
+      </c>
+      <c r="B8" t="s">
+        <v>479</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización del aislador USB
</commit_message>
<xml_diff>
--- a/Librería de componentes.xlsx
+++ b/Librería de componentes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YUNELY\Desktop\ITLA\Décimo segundo cuatrimestre\Electiva Mecatrónica - Diseño Mecatrónico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0A2AE2-DE3F-49ED-AF3A-42286E71340F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A3DF62-069F-41D3-933A-A6DCE212D77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="5" xr2:uid="{49458E5D-DEEC-430E-940B-19D27B1F3765}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="7" xr2:uid="{49458E5D-DEEC-430E-940B-19D27B1F3765}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistencias" sheetId="1" r:id="rId1"/>
@@ -8685,7 +8685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A95F01-B128-436C-9F73-5C18FF680B8D}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
@@ -9495,9 +9495,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45386E3-6834-48BE-9DB4-36059B842F86}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9692,7 +9692,7 @@
         <v>489</v>
       </c>
       <c r="G8" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -9761,7 +9761,7 @@
         <v>489</v>
       </c>
       <c r="G11" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -9830,7 +9830,7 @@
         <v>489</v>
       </c>
       <c r="G14" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -9922,7 +9922,7 @@
         <v>489</v>
       </c>
       <c r="G18" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -10014,7 +10014,7 @@
         <v>489</v>
       </c>
       <c r="G22" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -10060,7 +10060,7 @@
         <v>489</v>
       </c>
       <c r="G24" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Librería de componentes y archivo de requisitos del proyecto
</commit_message>
<xml_diff>
--- a/Librería de componentes.xlsx
+++ b/Librería de componentes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YUNELY\Desktop\ITLA\Décimo segundo cuatrimestre\Electiva Mecatrónica - Diseño Mecatrónico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A3DF62-069F-41D3-933A-A6DCE212D77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61EC8EBB-BB71-4BB2-B923-6C6700CE0990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="7" xr2:uid="{49458E5D-DEEC-430E-940B-19D27B1F3765}"/>
   </bookViews>
@@ -9496,8 +9496,8 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9692,7 +9692,7 @@
         <v>489</v>
       </c>
       <c r="G8" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -9738,7 +9738,7 @@
         <v>489</v>
       </c>
       <c r="G10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -10014,7 +10014,7 @@
         <v>489</v>
       </c>
       <c r="G22" s="10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -10106,7 +10106,7 @@
         <v>489</v>
       </c>
       <c r="G26" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -10129,7 +10129,7 @@
         <v>489</v>
       </c>
       <c r="G27" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>